<commit_message>
soc2 rev 2022 as a separate library
</commit_message>
<xml_diff>
--- a/tools/aicpa/SOC2_2017_with_rev_2022.xlsx
+++ b/tools/aicpa/SOC2_2017_with_rev_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thida\Downloads\CISO ASSISTANT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/aicpa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B58311F-31BE-4BC7-8D5B-90942F4A67F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9007135F-3C7A-5843-BB74-9919D0DC2F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D01D941C-8F4B-437A-8397-2B749EA54579}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" xr2:uid="{D01D941C-8F4B-437A-8397-2B749EA54579}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="1180">
   <si>
     <t>System Operations</t>
   </si>
@@ -3631,6 +3631,9 @@
     <t>TSP Sección 100
 2017 Trust Services Criteria for Security, Availability, Processing Integrity, Confidentiality, and Privacy (con puntos de atención revisados - 2022)
 TSC presenta criterios de control establecidos por el Comité Ejecutivo de Servicios de Aseguramiento (ASEC) del AICPA para su uso en compromisos de atestación o consultoría para evaluar e informar sobre los controles sobre la seguridad, disponibilidad, integridad de procesamiento, confidencialidad o privacidad de la información y los sistemas utilizados para proporcionar productos o servicios (a) en toda una entidad; (b) a nivel de subsidiaria, división o unidad operativa; (c) dentro de una función relevante para los objetivos operativos, de información o de cumplimiento de la entidad; y (d) para un tipo particular de información utilizada por la entidad. Link: https://www.aicpa-cima.com/resources/download/2017-trust-services-criteria-with-revised-points-of-focus-2022</t>
+  </si>
+  <si>
+    <t>library_publication_date</t>
   </si>
 </sst>
 </file>
@@ -3753,7 +3756,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3833,7 +3836,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3843,8 +3846,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3864,12 +3870,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -4165,17 +4167,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951F4425-FB26-465D-A91F-BEC42F32E716}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110.85546875" style="29" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="29"/>
+    <col min="2" max="2" width="110.83203125" style="29" customWidth="1"/>
+    <col min="3" max="16384" width="11.5" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -4223,7 +4225,7 @@
       </c>
       <c r="C5" s="31"/>
     </row>
-    <row r="6" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>1147</v>
       </c>
@@ -4232,7 +4234,7 @@
       </c>
       <c r="C6" s="31"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
         <v>1148</v>
       </c>
@@ -4260,89 +4262,98 @@
       <c r="C9" s="31"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="33" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B10" s="36">
+        <v>45199</v>
+      </c>
+      <c r="C10" s="31"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="30" t="s">
         <v>1154</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B11" s="31" t="s">
         <v>1164</v>
       </c>
-      <c r="C10" s="31"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="C11" s="31"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
         <v>1155</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B12" s="31" t="s">
         <v>1162</v>
       </c>
-      <c r="C11" s="31"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="C12" s="31"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
         <v>1156</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B13" s="31" t="s">
         <v>1146</v>
       </c>
-      <c r="C12" s="31"/>
-    </row>
-    <row r="13" spans="1:3" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+      <c r="C13" s="31"/>
+    </row>
+    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
         <v>1157</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B14" s="34" t="s">
         <v>1163</v>
       </c>
-      <c r="C13" s="31"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
         <v>1158</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B15" s="31" t="s">
         <v>1159</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C15" s="31" t="s">
         <v>1160</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>1165</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B16" s="31" t="s">
         <v>1146</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+    <row r="17" spans="1:2" ht="120" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
         <v>1166</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B17" s="35" t="s">
         <v>1178</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
         <v>1167</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B18" s="34" t="s">
         <v>1149</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>1162</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
         <v>1169</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B20" s="31" t="s">
         <v>1146</v>
       </c>
     </row>
@@ -4361,18 +4372,18 @@
       <selection pane="bottomLeft" activeCell="B319" sqref="B319"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="15" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="15" customWidth="1"/>
     <col min="4" max="4" width="30" style="15" customWidth="1"/>
-    <col min="5" max="5" width="88.140625" customWidth="1"/>
+    <col min="5" max="5" width="88.1640625" customWidth="1"/>
     <col min="6" max="6" width="56" customWidth="1"/>
-    <col min="7" max="7" width="95.28515625" customWidth="1"/>
+    <col min="7" max="7" width="95.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>1059</v>
       </c>
@@ -4395,7 +4406,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="22">
         <v>1</v>
@@ -4410,7 +4421,7 @@
       </c>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="6">
         <v>2</v>
@@ -4431,7 +4442,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4450,7 +4461,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4469,7 +4480,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4488,7 +4499,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4507,7 +4518,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4526,7 +4537,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6">
         <v>2</v>
@@ -4547,7 +4558,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4566,7 +4577,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4585,7 +4596,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4604,7 +4615,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4623,7 +4634,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <v>2</v>
@@ -4644,7 +4655,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4663,7 +4674,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4682,7 +4693,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4701,7 +4712,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4720,7 +4731,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4739,7 +4750,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4758,7 +4769,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6">
         <v>2</v>
@@ -4779,7 +4790,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4798,7 +4809,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4817,7 +4828,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4836,7 +4847,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4855,7 +4866,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4874,7 +4885,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4893,7 +4904,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4912,7 +4923,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6">
         <v>2</v>
@@ -4933,7 +4944,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4952,7 +4963,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4971,7 +4982,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>1139</v>
       </c>
@@ -4990,7 +5001,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5009,7 +5020,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5028,7 +5039,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5047,7 +5058,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="22"/>
       <c r="B36" s="22">
         <v>1</v>
@@ -5062,7 +5073,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4">
         <v>2</v>
@@ -5083,7 +5094,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5102,7 +5113,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5121,7 +5132,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5140,7 +5151,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5159,7 +5170,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5178,7 +5189,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5197,7 +5208,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5216,7 +5227,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5235,7 +5246,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5254,7 +5265,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4">
         <v>2</v>
@@ -5275,7 +5286,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5294,7 +5305,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5313,7 +5324,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5332,7 +5343,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5351,7 +5362,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5370,7 +5381,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5389,7 +5400,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5408,7 +5419,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5427,7 +5438,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5446,7 +5457,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5465,7 +5476,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5484,7 +5495,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5503,7 +5514,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5522,7 +5533,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4">
         <v>2</v>
@@ -5543,7 +5554,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5562,7 +5573,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5581,7 +5592,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5600,7 +5611,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5619,7 +5630,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5638,7 +5649,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5657,7 +5668,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5676,7 +5687,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5695,7 +5706,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5714,7 +5725,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5733,7 +5744,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5752,7 +5763,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>1139</v>
       </c>
@@ -5771,7 +5782,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="26"/>
       <c r="B74" s="26">
         <v>1</v>
@@ -5786,7 +5797,7 @@
       </c>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
       <c r="B75" s="6">
         <v>2</v>
@@ -5807,7 +5818,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5826,7 +5837,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5845,7 +5856,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5864,7 +5875,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5883,7 +5894,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5902,7 +5913,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5921,7 +5932,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5940,7 +5951,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5959,7 +5970,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5978,7 +5989,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>1139</v>
       </c>
@@ -5997,7 +6008,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6016,7 +6027,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6035,7 +6046,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6054,7 +6065,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6073,7 +6084,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6092,7 +6103,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6111,7 +6122,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="6"/>
       <c r="B92" s="6">
         <v>2</v>
@@ -6132,7 +6143,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6151,7 +6162,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6170,7 +6181,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6189,7 +6200,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6208,7 +6219,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6227,7 +6238,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6246,7 +6257,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6265,7 +6276,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6284,7 +6295,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="6"/>
       <c r="B101" s="6">
         <v>2</v>
@@ -6305,7 +6316,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6324,7 +6335,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6343,7 +6354,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6362,7 +6373,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6381,7 +6392,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6400,7 +6411,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="6"/>
       <c r="B107" s="6">
         <v>2</v>
@@ -6421,7 +6432,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6440,7 +6451,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6459,7 +6470,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6478,7 +6489,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6497,7 +6508,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6516,7 +6527,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6535,7 +6546,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="22"/>
       <c r="B114" s="22">
         <v>1</v>
@@ -6550,7 +6561,7 @@
       </c>
       <c r="G114" s="3"/>
     </row>
-    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="6"/>
       <c r="B115" s="6">
         <v>2</v>
@@ -6571,7 +6582,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6590,7 +6601,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6609,7 +6620,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6628,7 +6639,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6647,7 +6658,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6666,7 +6677,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6685,7 +6696,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6704,7 +6715,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6723,7 +6734,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="6"/>
       <c r="B124" s="6">
         <v>2</v>
@@ -6744,7 +6755,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6763,7 +6774,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6782,7 +6793,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6801,7 +6812,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="22"/>
       <c r="B128" s="22">
         <v>1</v>
@@ -6816,7 +6827,7 @@
       </c>
       <c r="G128" s="2"/>
     </row>
-    <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="6"/>
       <c r="B129" s="6">
         <v>2</v>
@@ -6837,7 +6848,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6856,7 +6867,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6875,7 +6886,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6894,7 +6905,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6913,7 +6924,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6932,7 +6943,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6951,7 +6962,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="6"/>
       <c r="B136" s="6">
         <v>2</v>
@@ -6972,7 +6983,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
         <v>1139</v>
       </c>
@@ -6991,7 +7002,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7010,7 +7021,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A139" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7029,7 +7040,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7048,7 +7059,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="6"/>
       <c r="B141" s="6">
         <v>2</v>
@@ -7067,7 +7078,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7086,7 +7097,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7105,7 +7116,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7124,7 +7135,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7143,7 +7154,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7162,7 +7173,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
         <v>1139</v>
       </c>
@@ -7181,7 +7192,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="22"/>
       <c r="B148" s="22">
         <v>1</v>
@@ -7196,7 +7207,7 @@
       </c>
       <c r="G148" s="3"/>
     </row>
-    <row r="149" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="4"/>
       <c r="B149" s="4">
         <v>2</v>
@@ -7213,7 +7224,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7232,7 +7243,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7251,7 +7262,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7270,7 +7281,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7289,7 +7300,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7308,7 +7319,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7327,7 +7338,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7346,7 +7357,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7365,7 +7376,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7384,7 +7395,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7403,7 +7414,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7422,7 +7433,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7441,7 +7452,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7460,7 +7471,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A163" s="4"/>
       <c r="B163" s="4">
         <v>2</v>
@@ -7477,7 +7488,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7496,7 +7507,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7515,7 +7526,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7534,7 +7545,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A167" s="4"/>
       <c r="B167" s="4">
         <v>2</v>
@@ -7551,7 +7562,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7570,7 +7581,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7589,7 +7600,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7608,7 +7619,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7627,7 +7638,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A172" s="4"/>
       <c r="B172" s="4">
         <v>2</v>
@@ -7644,7 +7655,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7663,7 +7674,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7682,7 +7693,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7701,7 +7712,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7720,7 +7731,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A177" s="4"/>
       <c r="B177" s="4">
         <v>2</v>
@@ -7737,7 +7748,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7756,7 +7767,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="4"/>
       <c r="B179" s="4">
         <v>2</v>
@@ -7773,7 +7784,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7792,7 +7803,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7811,7 +7822,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7830,7 +7841,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7849,7 +7860,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A184" s="4"/>
       <c r="B184" s="4">
         <v>2</v>
@@ -7866,7 +7877,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7885,7 +7896,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7904,7 +7915,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7923,7 +7934,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7942,7 +7953,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="4"/>
       <c r="B189" s="4">
         <v>2</v>
@@ -7959,7 +7970,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7978,7 +7989,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>1139</v>
       </c>
@@ -7997,7 +8008,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>1139</v>
       </c>
@@ -8016,7 +8027,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
         <v>1139</v>
       </c>
@@ -8035,7 +8046,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>1139</v>
       </c>
@@ -8054,7 +8065,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="26"/>
       <c r="B195" s="26">
         <v>1</v>
@@ -8069,7 +8080,7 @@
       </c>
       <c r="G195" s="3"/>
     </row>
-    <row r="196" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A196" s="6"/>
       <c r="B196" s="6">
         <v>2</v>
@@ -8086,7 +8097,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8105,7 +8116,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8124,7 +8135,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8143,7 +8154,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8162,7 +8173,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8181,7 +8192,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A202" s="6"/>
       <c r="B202" s="6">
         <v>2</v>
@@ -8198,7 +8209,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8217,7 +8228,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A204" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8236,7 +8247,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8255,7 +8266,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8274,7 +8285,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="207" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A207" s="6"/>
       <c r="B207" s="6">
         <v>2</v>
@@ -8291,7 +8302,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8310,7 +8321,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A209" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8329,7 +8340,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8348,7 +8359,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8367,7 +8378,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A212" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8386,7 +8397,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A213" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8405,7 +8416,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A214" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8424,7 +8435,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="6"/>
       <c r="B215" s="6">
         <v>2</v>
@@ -8441,7 +8452,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A216" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8460,7 +8471,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A217" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8479,7 +8490,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8498,7 +8509,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8517,7 +8528,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8536,7 +8547,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A221" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8555,7 +8566,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A222" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8574,7 +8585,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8593,7 +8604,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8612,7 +8623,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8631,7 +8642,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A226" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8650,7 +8661,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A227" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8669,7 +8680,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A228" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8688,7 +8699,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A229" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8707,7 +8718,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="6"/>
       <c r="B230" s="6">
         <v>2</v>
@@ -8724,7 +8735,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A231" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8743,7 +8754,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8762,7 +8773,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8781,7 +8792,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A234" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8800,7 +8811,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8819,7 +8830,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8838,7 +8849,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A237" s="22"/>
       <c r="B237" s="22">
         <v>1</v>
@@ -8853,7 +8864,7 @@
       </c>
       <c r="G237" s="3"/>
     </row>
-    <row r="238" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="6"/>
       <c r="B238" s="6">
         <v>2</v>
@@ -8870,7 +8881,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A239" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8889,7 +8900,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A240" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8908,7 +8919,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A241" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8927,7 +8938,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A242" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8946,7 +8957,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A243" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8965,7 +8976,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A244" s="6" t="s">
         <v>1139</v>
       </c>
@@ -8984,7 +8995,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A245" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9003,7 +9014,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A246" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9022,7 +9033,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A247" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9041,7 +9052,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A248" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9060,7 +9071,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A249" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9079,7 +9090,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A250" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9098,7 +9109,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A251" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9117,7 +9128,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A252" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9136,7 +9147,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A253" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9155,7 +9166,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A254" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9174,7 +9185,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A255" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9193,7 +9204,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A256" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9212,7 +9223,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A257" s="22"/>
       <c r="B257" s="22">
         <v>1</v>
@@ -9227,7 +9238,7 @@
       </c>
       <c r="G257" s="3"/>
     </row>
-    <row r="258" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A258" s="6"/>
       <c r="B258" s="6">
         <v>2</v>
@@ -9244,7 +9255,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="259" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A259" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9263,7 +9274,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="260" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A260" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9282,7 +9293,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A261" s="6"/>
       <c r="B261" s="6">
         <v>2</v>
@@ -9299,7 +9310,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A262" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9318,7 +9329,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A263" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9337,7 +9348,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A264" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9356,7 +9367,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A265" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9375,7 +9386,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A266" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9394,7 +9405,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="267" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A267" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9413,7 +9424,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="268" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A268" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9432,7 +9443,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="269" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A269" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9451,7 +9462,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="270" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A270" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9470,7 +9481,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="271" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A271" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9489,7 +9500,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A272" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9508,7 +9519,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="273" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A273" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9527,7 +9538,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="274" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A274" s="6" t="s">
         <v>1139</v>
       </c>
@@ -9546,7 +9557,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="275" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A275" s="22"/>
       <c r="B275" s="22">
         <v>1</v>
@@ -9560,7 +9571,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="276" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A276" s="4"/>
       <c r="B276" s="4">
         <v>2</v>
@@ -9577,7 +9588,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="277" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A277" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9596,7 +9607,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="278" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A278" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9615,7 +9626,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="279" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A279" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9634,7 +9645,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="280" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A280" s="4"/>
       <c r="B280" s="4">
         <v>2</v>
@@ -9651,7 +9662,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="281" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A281" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9670,7 +9681,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="282" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A282" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9689,7 +9700,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="283" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A283" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9708,7 +9719,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="284" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A284" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9727,7 +9738,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="285" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A285" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9746,7 +9757,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="286" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A286" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9765,7 +9776,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="287" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A287" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9784,7 +9795,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="288" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A288" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9803,7 +9814,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="289" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A289" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9822,7 +9833,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="290" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A290" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9841,7 +9852,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="291" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A291" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9860,7 +9871,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="292" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="4"/>
       <c r="B292" s="4">
         <v>2</v>
@@ -9877,7 +9888,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="293" spans="1:7" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9896,7 +9907,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="294" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A294" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9915,7 +9926,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="295" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A295" s="26"/>
       <c r="B295" s="26">
         <v>1</v>
@@ -9930,7 +9941,7 @@
       </c>
       <c r="G295" s="3"/>
     </row>
-    <row r="296" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A296" s="4"/>
       <c r="B296" s="4">
         <v>2</v>
@@ -9947,7 +9958,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="297" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A297" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9966,7 +9977,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="298" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A298" s="4" t="s">
         <v>1139</v>
       </c>
@@ -9985,7 +9996,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="299" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A299" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10004,7 +10015,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="300" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A300" s="4"/>
       <c r="B300" s="4">
         <v>2</v>
@@ -10021,7 +10032,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="301" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A301" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10040,7 +10051,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="302" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A302" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10059,7 +10070,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="303" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A303" s="26"/>
       <c r="B303" s="26">
         <v>1</v>
@@ -10074,7 +10085,7 @@
       </c>
       <c r="G303" s="3"/>
     </row>
-    <row r="304" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10093,7 +10104,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="305" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A305" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10112,7 +10123,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="306" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A306" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10131,7 +10142,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="307" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10150,7 +10161,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="308" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A308" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10169,7 +10180,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A309" s="26"/>
       <c r="B309" s="26">
         <v>1</v>
@@ -10184,7 +10195,7 @@
       </c>
       <c r="G309" s="3"/>
     </row>
-    <row r="310" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10203,7 +10214,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="311" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A311" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10222,7 +10233,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A312" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10241,7 +10252,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="313" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A313" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10260,7 +10271,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A314" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10279,7 +10290,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="315" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10298,7 +10309,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="316" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A316" s="4"/>
       <c r="B316" s="4">
         <v>3</v>
@@ -10315,7 +10326,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="317" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A317" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10334,7 +10345,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="318" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A318" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10353,7 +10364,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A319" s="4"/>
       <c r="B319" s="4">
         <v>2</v>
@@ -10370,7 +10381,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="320" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A320" s="4"/>
       <c r="B320" s="4">
         <v>3</v>
@@ -10387,7 +10398,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="321" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A321" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10406,7 +10417,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="322" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A322" s="4"/>
       <c r="B322" s="4">
         <v>3</v>
@@ -10423,7 +10434,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="323" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A323" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10442,7 +10453,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="324" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A324" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10461,7 +10472,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="325" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A325" s="4"/>
       <c r="B325" s="4">
         <v>3</v>
@@ -10478,7 +10489,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="326" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A326" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10497,7 +10508,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="327" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A327" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10516,7 +10527,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="328" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A328" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10535,7 +10546,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A329" s="4"/>
       <c r="B329" s="4">
         <v>2</v>
@@ -10552,7 +10563,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="330" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A330" s="4"/>
       <c r="B330" s="4">
         <v>3</v>
@@ -10569,7 +10580,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="331" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A331" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10588,7 +10599,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="332" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A332" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10607,7 +10618,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="333" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A333" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10626,7 +10637,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="334" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A334" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10645,7 +10656,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="335" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A335" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10664,7 +10675,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="336" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A336" s="4"/>
       <c r="B336" s="4">
         <v>3</v>
@@ -10681,7 +10692,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="337" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A337" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10700,7 +10711,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="338" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A338" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10719,7 +10730,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="339" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A339" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10738,7 +10749,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="340" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A340" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10757,7 +10768,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A341" s="4"/>
       <c r="B341" s="4">
         <v>2</v>
@@ -10774,7 +10785,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="342" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A342" s="4"/>
       <c r="B342" s="4">
         <v>3</v>
@@ -10791,7 +10802,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="343" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A343" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10810,7 +10821,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="344" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A344" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10829,7 +10840,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="345" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A345" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10848,7 +10859,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="346" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A346" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10867,7 +10878,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="347" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A347" s="4"/>
       <c r="B347" s="4">
         <v>3</v>
@@ -10884,7 +10895,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="348" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A348" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10903,7 +10914,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="349" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A349" s="4"/>
       <c r="B349" s="4">
         <v>3</v>
@@ -10920,7 +10931,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A350" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10939,7 +10950,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="351" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A351" s="4"/>
       <c r="B351" s="4">
         <v>3</v>
@@ -10956,7 +10967,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="352" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A352" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10975,7 +10986,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="353" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A353" s="4" t="s">
         <v>1139</v>
       </c>
@@ -10994,7 +11005,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="354" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A354" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11013,7 +11024,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="355" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A355" s="4"/>
       <c r="B355" s="4">
         <v>3</v>
@@ -11030,7 +11041,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="356" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A356" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11049,7 +11060,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="357" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A357" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11068,7 +11079,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="358" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A358" s="4"/>
       <c r="B358" s="4">
         <v>3</v>
@@ -11085,7 +11096,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="359" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A359" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11104,7 +11115,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="360" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A360" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11123,7 +11134,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="361" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A361" s="4"/>
       <c r="B361" s="4">
         <v>3</v>
@@ -11140,7 +11151,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="362" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A362" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11159,7 +11170,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="363" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A363" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11178,7 +11189,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="364" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A364" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11197,7 +11208,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A365" s="4"/>
       <c r="B365" s="4">
         <v>2</v>
@@ -11214,7 +11225,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="366" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A366" s="4"/>
       <c r="B366" s="4">
         <v>3</v>
@@ -11231,7 +11242,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="367" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A367" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11250,7 +11261,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="368" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A368" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11269,7 +11280,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A369" s="4"/>
       <c r="B369" s="4">
         <v>2</v>
@@ -11286,7 +11297,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="370" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A370" s="4"/>
       <c r="B370" s="4">
         <v>3</v>
@@ -11303,7 +11314,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="371" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A371" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11322,7 +11333,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="372" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A372" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11341,7 +11352,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="373" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A373" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11360,7 +11371,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="374" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A374" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11379,7 +11390,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="375" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A375" s="4" t="s">
         <v>1139</v>
       </c>
@@ -11398,7 +11409,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="376" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A376" s="4" t="s">
         <v>1139</v>
       </c>

</xml_diff>

<commit_message>
change title for SOC2 2017 revision 2022 (#1353)
change title
</commit_message>
<xml_diff>
--- a/tools/aicpa/SOC2_2017_with_rev_2022.xlsx
+++ b/tools/aicpa/SOC2_2017_with_rev_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/aicpa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C2C304-3412-F846-8971-2220FF7A7628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0636A7-AB61-9442-BA3D-3D4AFC5722EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="500" windowWidth="34240" windowHeight="20580" xr2:uid="{D01D941C-8F4B-437A-8397-2B749EA54579}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="1193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="1194">
   <si>
     <t>System Operations</t>
   </si>
@@ -3673,6 +3673,9 @@
   </si>
   <si>
     <t>CC5</t>
+  </si>
+  <si>
+    <t>SOC2-2017 Trust Services Criteria (revision 2022)</t>
   </si>
 </sst>
 </file>
@@ -4209,7 +4212,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -4260,7 +4263,7 @@
         <v>1144</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>1145</v>
+        <v>1193</v>
       </c>
       <c r="C5" s="31"/>
     </row>
@@ -4332,7 +4335,7 @@
         <v>1155</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>1145</v>
+        <v>1193</v>
       </c>
       <c r="C13" s="31"/>
     </row>

</xml_diff>